<commit_message>
Updated BOM to fix DNI/DNS typos.
</commit_message>
<xml_diff>
--- a/PCB/eZ_Navi-Delete_BOM.xlsx
+++ b/PCB/eZ_Navi-Delete_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\KiCAD\eZ_HW_v1p0b-STM32_DC-DC_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\github\eZ_Navi-Delete\trunk\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AFE8FE7-44D4-4BA1-98EB-7791358B83CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C178C785-8BEF-4B33-B10C-A9313FAC1020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1468,7 +1468,7 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,7 +1924,7 @@
         <v>63</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>64</v>
@@ -1939,7 +1939,7 @@
         <v>67</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1950,7 +1950,7 @@
         <v>68</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>64</v>
@@ -1965,7 +1965,7 @@
         <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1976,7 +1976,7 @@
         <v>72</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
@@ -1991,7 +1991,7 @@
         <v>75</v>
       </c>
       <c r="H20" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>